<commit_message>
Update: Python, Python packages, 改善点リスト
</commit_message>
<xml_diff>
--- a/設計・実験/設計メモ.xlsx
+++ b/設計・実験/設計メモ.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@VBRT-NOCHK\!G\repos\pyscreenshot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@VBRT-NOCHK\!G\repos\pyscreenshot\設計・実験\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14851060-8C8F-4B6D-AFA7-2E4AE54E03D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44014F32-0936-4A4C-B447-45052A789916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="660" windowWidth="24000" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="240" windowWidth="24855" windowHeight="15105" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="機能と実装状況" sheetId="3" r:id="rId1"/>
     <sheet name="設定項目（プロパティ）" sheetId="1" r:id="rId2"/>
     <sheet name="ホット・キーについて" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="243">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -1685,6 +1686,66 @@
     <t>⑧[PNGファイルへ保存]</t>
     <rPh sb="10" eb="12">
       <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■改善項目</t>
+    <rPh sb="1" eb="3">
+      <t>カイゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウモク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1. 途中で以前のキャプチャー画像を削除した場合に、シーケンス番号の空きを見つけていない。</t>
+    <rPh sb="3" eb="5">
+      <t>トチュウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>イゼン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2. 現在保持している「次のシーケンス番号」をリセットする手段が欲しい。</t>
+    <rPh sb="3" eb="5">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>シュダン</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ホ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3664,7 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -5729,4 +5790,38 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BFFC8D-D8FF-4489-BB17-507B878805B6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>